<commit_message>
adding commands and branch theroy
</commit_message>
<xml_diff>
--- a/Trackers/Atendance tracker.xlsx
+++ b/Trackers/Atendance tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SourceandCode\Source_code_batch_4\Trackers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C429E534-957C-4CD1-8A64-B1731330AAFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502A55C9-BCC4-4170-9209-E15D2160ADBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A32A0B54-107B-49F7-862C-6CFC80B9902E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="16">
   <si>
     <t>SR NO</t>
   </si>
@@ -531,8 +531,8 @@
   <dimension ref="A1:AH11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F12" sqref="F12"/>
+      <pane xSplit="2" topLeftCell="AF1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AH13" sqref="AH13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,13 +666,16 @@
       <c r="D2" t="s">
         <v>13</v>
       </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
       <c r="AG2">
         <f>COUNTIF(C2:AF2,"PRESENT")</f>
         <v>1</v>
       </c>
       <c r="AH2">
-        <f>COUNTIF(C2:AF2,"PRESENT")/COUNTA(C2:AF2)</f>
-        <v>0.5</v>
+        <f>COUNTIF(C2:AF2,"PRESENT")/COUNTA(C2:AF2)*100</f>
+        <v>33.333333333333329</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.3">
@@ -688,13 +691,16 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
       <c r="AG3">
         <f t="shared" ref="AG3:AG11" si="0">COUNTIF(C3:AF3,"PRESENT")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH3">
-        <f>COUNTIF(C2:AF2,"PRESENT")/COUNTA(C2:AF2)</f>
-        <v>0.5</v>
+        <f t="shared" ref="AH3:AH11" si="1">COUNTIF(C3:AF3,"PRESENT")/COUNTA(C3:AF3)*100</f>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.3">
@@ -710,13 +716,16 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
       <c r="AG4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH4">
-        <f t="shared" ref="AH4:AH11" si="1">COUNTIF(C3:AF3,"PRESENT")/COUNTA(C3:AF3)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.3">
@@ -732,13 +741,16 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
       <c r="AG5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.3">
@@ -754,13 +766,16 @@
       <c r="D6" t="s">
         <v>12</v>
       </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
       <c r="AG6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH6">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.3">
@@ -776,13 +791,16 @@
       <c r="D7" t="s">
         <v>12</v>
       </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
       <c r="AG7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.3">
@@ -798,13 +816,16 @@
       <c r="D8" t="s">
         <v>12</v>
       </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
       <c r="AG8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH8">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.3">
@@ -820,13 +841,16 @@
       <c r="D9" t="s">
         <v>12</v>
       </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
       <c r="AG9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH9">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.3">
@@ -842,13 +866,16 @@
       <c r="D10" t="s">
         <v>13</v>
       </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
       <c r="AG10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AH10">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.3">
@@ -862,6 +889,9 @@
         <v>13</v>
       </c>
       <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
         <v>13</v>
       </c>
       <c r="AG11">
@@ -899,8 +929,8 @@
   <dimension ref="A1:AH11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I7" sqref="I7"/>
+      <pane xSplit="2" topLeftCell="AE1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AJ5" sqref="AJ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1032,7 +1062,7 @@
         <v>0</v>
       </c>
       <c r="AH2">
-        <f>COUNTIF(C2:AF2,"PRESENT")/COUNTA(C2:AF2)</f>
+        <f>COUNTIF(C2:AF2,"PRESENT")/COUNTA(C2:AF2)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -1054,8 +1084,8 @@
         <v>2</v>
       </c>
       <c r="AH3">
-        <f t="shared" ref="AH3:AH11" si="1">COUNTIF(C3:AF3,"PRESENT")/COUNTA(C3:AF3)</f>
-        <v>1</v>
+        <f t="shared" ref="AH3:AH11" si="1">COUNTIF(C3:AF3,"PRESENT")/COUNTA(C3:AF3)*100</f>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:34" ht="27" x14ac:dyDescent="0.3">
@@ -1077,7 +1107,7 @@
       </c>
       <c r="AH4">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:34" ht="27" x14ac:dyDescent="0.3">
@@ -1099,7 +1129,7 @@
       </c>
       <c r="AH5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:34" ht="27" x14ac:dyDescent="0.3">
@@ -1121,7 +1151,7 @@
       </c>
       <c r="AH6">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:34" ht="53.4" x14ac:dyDescent="0.3">
@@ -1143,7 +1173,7 @@
       </c>
       <c r="AH7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:34" ht="27" x14ac:dyDescent="0.3">
@@ -1187,7 +1217,7 @@
       </c>
       <c r="AH9">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
support session for PR raise
</commit_message>
<xml_diff>
--- a/Trackers/Atendance tracker.xlsx
+++ b/Trackers/Atendance tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SourceandCode\Source_code_batch_4\Trackers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71AB63A-911E-4267-A689-C9669B0FB36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733C8E72-E565-44F1-B580-4CFDD52E8D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A32A0B54-107B-49F7-862C-6CFC80B9902E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="16">
   <si>
     <t>SR NO</t>
   </si>
@@ -90,7 +90,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,13 +112,26 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -148,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -163,6 +176,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,7 +546,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H20" sqref="H20"/>
+      <selection pane="topRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -700,9 +714,12 @@
       <c r="F3" t="s">
         <v>12</v>
       </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
       <c r="AG3">
         <f t="shared" ref="AG3:AG11" si="0">COUNTIF(C3:AF3,"PRESENT")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH3">
         <f t="shared" ref="AH3:AH11" si="1">COUNTIF(C3:AF3,"PRESENT")/COUNTA(C3:AF3)*100</f>
@@ -728,9 +745,12 @@
       <c r="F4" t="s">
         <v>12</v>
       </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
       <c r="AG4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH4">
         <f t="shared" si="1"/>
@@ -756,9 +776,12 @@
       <c r="F5" t="s">
         <v>12</v>
       </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
       <c r="AG5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH5">
         <f t="shared" si="1"/>
@@ -784,9 +807,12 @@
       <c r="F6" t="s">
         <v>12</v>
       </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
       <c r="AG6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH6">
         <f t="shared" si="1"/>
@@ -812,13 +838,16 @@
       <c r="F7" t="s">
         <v>12</v>
       </c>
+      <c r="G7" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="AG7">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="AH7">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.3">
@@ -840,13 +869,16 @@
       <c r="F8" t="s">
         <v>13</v>
       </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
       <c r="AG8">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH8">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.3">
@@ -868,9 +900,12 @@
       <c r="F9" t="s">
         <v>12</v>
       </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
       <c r="AG9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH9">
         <f t="shared" si="1"/>
@@ -896,6 +931,9 @@
       <c r="F10" t="s">
         <v>13</v>
       </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
       <c r="AG10">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -924,6 +962,9 @@
       <c r="F11" t="s">
         <v>13</v>
       </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
       <c r="AG11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -934,7 +975,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:AG11">
+  <conditionalFormatting sqref="C2:AG6 C8:AG11 C7:F7 H7:AG7">
     <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="ABSENT">
       <formula>NOT(ISERROR(SEARCH("ABSENT",C2)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Assignment on string added
</commit_message>
<xml_diff>
--- a/Trackers/Atendance tracker.xlsx
+++ b/Trackers/Atendance tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SourceandCode\Source_code_batch_4\Trackers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733C8E72-E565-44F1-B580-4CFDD52E8D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC8E8B1-94E7-4466-BEB1-A25C9548B9B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A32A0B54-107B-49F7-862C-6CFC80B9902E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="17">
   <si>
     <t>SR NO</t>
   </si>
@@ -85,6 +85,9 @@
   <si>
     <t>% Attendance</t>
   </si>
+  <si>
+    <t>WEEKEND HOLIDAY</t>
+  </si>
 </sst>
 </file>
 
@@ -120,7 +123,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,6 +134,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -161,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -177,11 +186,67 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF92D050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF92D050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF92D050"/>
@@ -546,7 +611,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H16" sqref="H16"/>
+      <selection pane="topRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,6 +624,7 @@
     <col min="7" max="7" width="14.88671875" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" customWidth="1"/>
     <col min="9" max="9" width="14.21875" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" customWidth="1"/>
     <col min="33" max="33" width="14.77734375" customWidth="1"/>
     <col min="34" max="34" width="16.5546875" customWidth="1"/>
   </cols>
@@ -585,10 +651,10 @@
       <c r="G1" s="6">
         <v>45905</v>
       </c>
-      <c r="H1" s="6">
+      <c r="H1" s="2">
         <v>45906</v>
       </c>
-      <c r="I1" s="6">
+      <c r="I1" s="2">
         <v>45907</v>
       </c>
       <c r="J1" s="6">
@@ -686,13 +752,23 @@
       <c r="F2" t="s">
         <v>12</v>
       </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="9"/>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
       <c r="AG2">
         <f>COUNTIF(C2:AF2,"PRESENT")</f>
         <v>2</v>
       </c>
       <c r="AH2">
         <f>COUNTIF(C2:AF2,"PRESENT")/COUNTA(C2:AF2)*100</f>
-        <v>50</v>
+        <v>28.571428571428569</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.3">
@@ -717,9 +793,14 @@
       <c r="G3" t="s">
         <v>12</v>
       </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" t="s">
+        <v>12</v>
+      </c>
       <c r="AG3">
         <f t="shared" ref="AG3:AG11" si="0">COUNTIF(C3:AF3,"PRESENT")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AH3">
         <f t="shared" ref="AH3:AH11" si="1">COUNTIF(C3:AF3,"PRESENT")/COUNTA(C3:AF3)*100</f>
@@ -748,9 +829,14 @@
       <c r="G4" t="s">
         <v>12</v>
       </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" t="s">
+        <v>12</v>
+      </c>
       <c r="AG4">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AH4">
         <f t="shared" si="1"/>
@@ -779,9 +865,14 @@
       <c r="G5" t="s">
         <v>12</v>
       </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" t="s">
+        <v>12</v>
+      </c>
       <c r="AG5">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AH5">
         <f t="shared" si="1"/>
@@ -810,9 +901,14 @@
       <c r="G6" t="s">
         <v>12</v>
       </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" t="s">
+        <v>12</v>
+      </c>
       <c r="AG6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AH6">
         <f t="shared" si="1"/>
@@ -841,13 +937,18 @@
       <c r="G7" s="8" t="s">
         <v>13</v>
       </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" t="s">
+        <v>12</v>
+      </c>
       <c r="AG7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH7">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>83.333333333333343</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.3">
@@ -872,13 +973,18 @@
       <c r="G8" t="s">
         <v>12</v>
       </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" t="s">
+        <v>13</v>
+      </c>
       <c r="AG8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="AH8">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>66.666666666666657</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.3">
@@ -903,9 +1009,14 @@
       <c r="G9" t="s">
         <v>12</v>
       </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" t="s">
+        <v>12</v>
+      </c>
       <c r="AG9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AH9">
         <f t="shared" si="1"/>
@@ -934,6 +1045,11 @@
       <c r="G10" t="s">
         <v>13</v>
       </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" t="s">
+        <v>13</v>
+      </c>
       <c r="AG10">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -965,6 +1081,11 @@
       <c r="G11" t="s">
         <v>13</v>
       </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" t="s">
+        <v>13</v>
+      </c>
       <c r="AG11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -975,12 +1096,26 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:AG6 C8:AG11 C7:F7 H7:AG7">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="ABSENT">
+  <mergeCells count="1">
+    <mergeCell ref="H2:I11"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C7:F7 C8:G11 C2:G6 J2:AG11">
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="ABSENT">
       <formula>NOT(ISERROR(SEARCH("ABSENT",C2)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="PRESENT">
+      <formula>NOT(ISERROR(SEARCH("PRESENT",C2)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+      <formula>PRESENT</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="ABSENT">
+      <formula>NOT(ISERROR(SEARCH("ABSENT",H2)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="PRESENT">
-      <formula>NOT(ISERROR(SEARCH("PRESENT",C2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("PRESENT",H2)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>PRESENT</formula>
@@ -1001,7 +1136,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G2" sqref="G2"/>
+      <selection pane="topRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1011,6 +1146,9 @@
     <col min="4" max="4" width="13.88671875" customWidth="1"/>
     <col min="5" max="5" width="20.77734375" customWidth="1"/>
     <col min="6" max="6" width="22.5546875" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" customWidth="1"/>
+    <col min="8" max="8" width="14.77734375" customWidth="1"/>
+    <col min="9" max="9" width="21.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.3">
@@ -1117,7 +1255,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1134,6 +1272,13 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" t="s">
         <v>13</v>
       </c>
       <c r="AG2">
@@ -1142,10 +1287,10 @@
       </c>
       <c r="AH2">
         <f>COUNTIF(C2:AF2,"PRESENT")/COUNTA(C2:AF2)*100</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" ht="27" x14ac:dyDescent="0.3">
+        <v>16.666666666666664</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1164,16 +1309,21 @@
       <c r="F3" t="s">
         <v>12</v>
       </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
       <c r="AG3">
         <f t="shared" ref="AG3:AG11" si="0">COUNTIF(C3:AF3,"PRESENT")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH3">
         <f t="shared" ref="AH3:AH11" si="1">COUNTIF(C3:AF3,"PRESENT")/COUNTA(C3:AF3)*100</f>
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1192,16 +1342,21 @@
       <c r="F4" t="s">
         <v>12</v>
       </c>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" t="s">
+        <v>12</v>
+      </c>
       <c r="AG4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH4">
         <f t="shared" si="1"/>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" ht="27" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1220,16 +1375,21 @@
       <c r="F5" t="s">
         <v>12</v>
       </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
       <c r="AG5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH5">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1248,16 +1408,21 @@
       <c r="F6" t="s">
         <v>12</v>
       </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" t="s">
+        <v>12</v>
+      </c>
       <c r="AG6">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH6">
         <f t="shared" si="1"/>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" ht="53.4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1276,16 +1441,21 @@
       <c r="F7" t="s">
         <v>12</v>
       </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" t="s">
+        <v>12</v>
+      </c>
       <c r="AG7">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH7">
         <f t="shared" si="1"/>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34" ht="27" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1302,6 +1472,11 @@
         <v>13</v>
       </c>
       <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" t="s">
         <v>13</v>
       </c>
       <c r="AG8">
@@ -1332,13 +1507,18 @@
       <c r="F9" t="s">
         <v>12</v>
       </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" t="s">
+        <v>12</v>
+      </c>
       <c r="AG9">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH9">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.3">
@@ -1360,6 +1540,11 @@
       <c r="F10" t="s">
         <v>13</v>
       </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" t="s">
+        <v>13</v>
+      </c>
       <c r="AG10">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1388,6 +1573,11 @@
       <c r="F11" t="s">
         <v>13</v>
       </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" t="s">
+        <v>13</v>
+      </c>
       <c r="AG11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1398,7 +1588,10 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:AG11">
+  <mergeCells count="1">
+    <mergeCell ref="G2:H11"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C3:F11 C2:G2 I2:AG11">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="ABSENT">
       <formula>NOT(ISERROR(SEARCH("ABSENT",C2)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
support session for Strings and folder structure
</commit_message>
<xml_diff>
--- a/Trackers/Atendance tracker.xlsx
+++ b/Trackers/Atendance tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SourceandCode\Source_code_batch_4\Trackers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC8E8B1-94E7-4466-BEB1-A25C9548B9B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B548A94F-9FE5-447A-A227-17B0E1CB13D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A32A0B54-107B-49F7-862C-6CFC80B9902E}"/>
+    <workbookView xWindow="3696" yWindow="3360" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{A32A0B54-107B-49F7-862C-6CFC80B9902E}"/>
   </bookViews>
   <sheets>
     <sheet name="Lecture Attendance Tracker" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="17">
   <si>
     <t>SR NO</t>
   </si>
@@ -186,42 +186,17 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF92D050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF92D050"/>
@@ -609,7 +584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B7792C5-B7BB-42C0-A798-F75287AB83FD}">
   <dimension ref="A1:AH11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="G15" sqref="G15"/>
     </sheetView>
@@ -755,10 +730,10 @@
       <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="9"/>
+      <c r="I2" s="10"/>
       <c r="J2" t="s">
         <v>13</v>
       </c>
@@ -793,8 +768,8 @@
       <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
       <c r="J3" t="s">
         <v>12</v>
       </c>
@@ -829,8 +804,8 @@
       <c r="G4" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
       <c r="J4" t="s">
         <v>12</v>
       </c>
@@ -865,8 +840,8 @@
       <c r="G5" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
       <c r="J5" t="s">
         <v>12</v>
       </c>
@@ -901,8 +876,8 @@
       <c r="G6" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
       <c r="J6" t="s">
         <v>12</v>
       </c>
@@ -937,8 +912,8 @@
       <c r="G7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
       <c r="J7" t="s">
         <v>12</v>
       </c>
@@ -973,8 +948,8 @@
       <c r="G8" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
       <c r="J8" t="s">
         <v>13</v>
       </c>
@@ -1009,8 +984,8 @@
       <c r="G9" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
       <c r="J9" t="s">
         <v>12</v>
       </c>
@@ -1045,8 +1020,8 @@
       <c r="G10" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
       <c r="J10" t="s">
         <v>13</v>
       </c>
@@ -1081,8 +1056,8 @@
       <c r="G11" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
       <c r="J11" t="s">
         <v>13</v>
       </c>
@@ -1099,14 +1074,14 @@
   <mergeCells count="1">
     <mergeCell ref="H2:I11"/>
   </mergeCells>
-  <conditionalFormatting sqref="C7:F7 C8:G11 C2:G6 J2:AG11">
-    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="ABSENT">
+  <conditionalFormatting sqref="C2:G6 J2:AG11 C7:F7 C8:G11">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="ABSENT">
       <formula>NOT(ISERROR(SEARCH("ABSENT",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="PRESENT">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="PRESENT">
       <formula>NOT(ISERROR(SEARCH("PRESENT",C2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>PRESENT</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1134,9 +1109,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A3D0880-F65B-45BF-ACAC-3EA58BAAB81B}">
   <dimension ref="A1:AH11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1149,6 +1124,7 @@
     <col min="7" max="7" width="13.44140625" customWidth="1"/>
     <col min="8" max="8" width="14.77734375" customWidth="1"/>
     <col min="9" max="9" width="21.77734375" customWidth="1"/>
+    <col min="10" max="10" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.3">
@@ -1274,11 +1250,14 @@
       <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="9"/>
+      <c r="H2" s="10"/>
       <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
         <v>13</v>
       </c>
       <c r="AG2">
@@ -1287,7 +1266,7 @@
       </c>
       <c r="AH2">
         <f>COUNTIF(C2:AF2,"PRESENT")/COUNTA(C2:AF2)*100</f>
-        <v>16.666666666666664</v>
+        <v>14.285714285714285</v>
       </c>
     </row>
     <row r="3" spans="1:34" ht="27" customHeight="1" x14ac:dyDescent="0.3">
@@ -1309,14 +1288,17 @@
       <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
       <c r="I3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" t="s">
         <v>12</v>
       </c>
       <c r="AG3">
         <f t="shared" ref="AG3:AG11" si="0">COUNTIF(C3:AF3,"PRESENT")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AH3">
         <f t="shared" ref="AH3:AH11" si="1">COUNTIF(C3:AF3,"PRESENT")/COUNTA(C3:AF3)*100</f>
@@ -1342,18 +1324,21 @@
       <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
       <c r="I4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" t="s">
         <v>12</v>
       </c>
       <c r="AG4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH4">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>83.333333333333343</v>
       </c>
     </row>
     <row r="5" spans="1:34" ht="27" customHeight="1" x14ac:dyDescent="0.3">
@@ -1375,14 +1360,17 @@
       <c r="F5" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
       <c r="I5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" t="s">
         <v>12</v>
       </c>
       <c r="AG5">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AH5">
         <f t="shared" si="1"/>
@@ -1408,18 +1396,21 @@
       <c r="F6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
       <c r="I6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" t="s">
         <v>12</v>
       </c>
       <c r="AG6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH6">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>83.333333333333343</v>
       </c>
     </row>
     <row r="7" spans="1:34" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1441,18 +1432,21 @@
       <c r="F7" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
       <c r="I7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" t="s">
         <v>12</v>
       </c>
       <c r="AG7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH7">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>83.333333333333343</v>
       </c>
     </row>
     <row r="8" spans="1:34" ht="27" customHeight="1" x14ac:dyDescent="0.3">
@@ -1474,9 +1468,12 @@
       <c r="F8" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
       <c r="I8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" t="s">
         <v>13</v>
       </c>
       <c r="AG8">
@@ -1507,18 +1504,21 @@
       <c r="F9" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
       <c r="I9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" t="s">
         <v>12</v>
       </c>
       <c r="AG9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH9">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>83.333333333333343</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.3">
@@ -1540,9 +1540,12 @@
       <c r="F10" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
       <c r="I10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" t="s">
         <v>13</v>
       </c>
       <c r="AG10">
@@ -1573,9 +1576,12 @@
       <c r="F11" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
       <c r="I11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" t="s">
         <v>13</v>
       </c>
       <c r="AG11">
@@ -1591,7 +1597,7 @@
   <mergeCells count="1">
     <mergeCell ref="G2:H11"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:F11 C2:G2 I2:AG11">
+  <conditionalFormatting sqref="C2:G2 C3:F11 I2:AG11">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="ABSENT">
       <formula>NOT(ISERROR(SEARCH("ABSENT",C2)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Support session on 16/08/2025
</commit_message>
<xml_diff>
--- a/Trackers/Atendance tracker.xlsx
+++ b/Trackers/Atendance tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SourceandCode\Source_code_batch_4\Trackers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3161555B-D08A-4753-AE23-404BAFEDBA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920C6F8F-9A7D-4FB4-95B5-7713D8B0830F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3696" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{A32A0B54-107B-49F7-862C-6CFC80B9902E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{A32A0B54-107B-49F7-862C-6CFC80B9902E}"/>
   </bookViews>
   <sheets>
     <sheet name="Lecture Attendance Tracker" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="33">
   <si>
     <t>SR NO</t>
   </si>
@@ -127,13 +127,22 @@
   </si>
   <si>
     <t>Pooja Patil</t>
+  </si>
+  <si>
+    <t>indrayanisuryawanshi.work@gmail.com</t>
+  </si>
+  <si>
+    <t>ankitafartade.work@gmail.com</t>
+  </si>
+  <si>
+    <t>Pooja</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,6 +195,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -314,10 +331,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -378,15 +396,194 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="51">
+    <dxf>
+      <font>
+        <color rgb="FF92D050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF92D050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF92D050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF92D050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF92D050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF92D050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF92D050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF92D050"/>
@@ -949,9 +1146,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B7792C5-B7BB-42C0-A798-F75287AB83FD}">
   <dimension ref="A1:AH13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AE1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C11" sqref="C11:G13"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -971,6 +1168,7 @@
     <col min="15" max="15" width="12.44140625" customWidth="1"/>
     <col min="16" max="16" width="15.109375" customWidth="1"/>
     <col min="17" max="17" width="17.109375" customWidth="1"/>
+    <col min="18" max="18" width="30.109375" customWidth="1"/>
     <col min="33" max="33" width="14.77734375" customWidth="1"/>
     <col min="34" max="34" width="16.5546875" customWidth="1"/>
   </cols>
@@ -1124,13 +1322,19 @@
         <v>16</v>
       </c>
       <c r="P2" s="19"/>
+      <c r="Q2" t="s">
+        <v>13</v>
+      </c>
+      <c r="R2" t="s">
+        <v>13</v>
+      </c>
       <c r="AG2">
         <f>COUNTIF(C2:AF2,"PRESENT")</f>
         <v>2</v>
       </c>
       <c r="AH2">
         <f>COUNTIF(C2:AF2,"PRESENT")/COUNTA(C2:AF2)*100</f>
-        <v>16.666666666666664</v>
+        <v>14.285714285714285</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.3">
@@ -1177,13 +1381,16 @@
       <c r="Q3" s="17" t="s">
         <v>12</v>
       </c>
+      <c r="R3" s="17" t="s">
+        <v>12</v>
+      </c>
       <c r="AG3">
         <f t="shared" ref="AG3:AG13" si="0">COUNTIF(C3:AF3,"PRESENT")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AH3">
         <f t="shared" ref="AH3:AH13" si="1">COUNTIF(C3:AF3,"PRESENT")/COUNTA(C3:AF3)*100</f>
-        <v>81.818181818181827</v>
+        <v>83.333333333333343</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.3">
@@ -1230,9 +1437,12 @@
       <c r="Q4" s="17" t="s">
         <v>12</v>
       </c>
+      <c r="R4" s="17" t="s">
+        <v>12</v>
+      </c>
       <c r="AG4">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AH4">
         <f t="shared" si="1"/>
@@ -1283,9 +1493,12 @@
       <c r="Q5" s="17" t="s">
         <v>12</v>
       </c>
+      <c r="R5" s="17" t="s">
+        <v>12</v>
+      </c>
       <c r="AG5">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AH5">
         <f t="shared" si="1"/>
@@ -1336,9 +1549,12 @@
       <c r="Q6" s="17" t="s">
         <v>12</v>
       </c>
+      <c r="R6" s="17" t="s">
+        <v>12</v>
+      </c>
       <c r="AG6">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AH6">
         <f t="shared" si="1"/>
@@ -1389,13 +1605,16 @@
       <c r="Q7" s="17" t="s">
         <v>12</v>
       </c>
+      <c r="R7" s="17" t="s">
+        <v>12</v>
+      </c>
       <c r="AG7">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AH7">
         <f t="shared" si="1"/>
-        <v>72.727272727272734</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.3">
@@ -1442,13 +1661,16 @@
       <c r="Q8" s="17" t="s">
         <v>12</v>
       </c>
+      <c r="R8" s="17" t="s">
+        <v>12</v>
+      </c>
       <c r="AG8">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AH8">
         <f t="shared" si="1"/>
-        <v>54.54545454545454</v>
+        <v>58.333333333333336</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.3">
@@ -1495,9 +1717,12 @@
       <c r="Q9" s="17" t="s">
         <v>12</v>
       </c>
+      <c r="R9" s="17" t="s">
+        <v>12</v>
+      </c>
       <c r="AG9">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AH9">
         <f t="shared" si="1"/>
@@ -1548,13 +1773,16 @@
       <c r="Q10" s="17" t="s">
         <v>12</v>
       </c>
+      <c r="R10" s="17" t="s">
+        <v>12</v>
+      </c>
       <c r="AG10">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AH10">
         <f t="shared" si="1"/>
-        <v>45.454545454545453</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.3">
@@ -1577,9 +1805,12 @@
       <c r="Q11" s="17" t="s">
         <v>12</v>
       </c>
+      <c r="R11" s="17" t="s">
+        <v>12</v>
+      </c>
       <c r="AG11">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH11">
         <f t="shared" si="1"/>
@@ -1606,20 +1837,23 @@
       <c r="Q12" t="s">
         <v>13</v>
       </c>
+      <c r="R12" s="17" t="s">
+        <v>12</v>
+      </c>
       <c r="AG12">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH12">
         <f t="shared" si="1"/>
-        <v>66.666666666666657</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A13" s="26">
-        <v>13</v>
-      </c>
-      <c r="B13" s="27" t="s">
+      <c r="A13" s="15">
+        <v>13</v>
+      </c>
+      <c r="B13" s="16" t="s">
         <v>29</v>
       </c>
       <c r="H13" s="19"/>
@@ -1635,9 +1869,12 @@
       <c r="Q13" s="17" t="s">
         <v>12</v>
       </c>
+      <c r="R13" s="17" t="s">
+        <v>12</v>
+      </c>
       <c r="AG13">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH13">
         <f t="shared" si="1"/>
@@ -1649,78 +1886,78 @@
     <mergeCell ref="O2:P13"/>
     <mergeCell ref="H2:I13"/>
   </mergeCells>
-  <conditionalFormatting sqref="C11:G12 J11:N12">
-    <cfRule type="containsText" dxfId="29" priority="13" operator="containsText" text="ABSENT">
-      <formula>NOT(ISERROR(SEARCH("ABSENT",C11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="14" operator="containsText" text="PRESENT">
-      <formula>NOT(ISERROR(SEARCH("PRESENT",C11)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="15" operator="equal">
+  <conditionalFormatting sqref="C8:G13">
+    <cfRule type="containsText" dxfId="50" priority="10" operator="containsText" text="ABSENT">
+      <formula>NOT(ISERROR(SEARCH("ABSENT",C8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="11" operator="containsText" text="PRESENT">
+      <formula>NOT(ISERROR(SEARCH("PRESENT",C8)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="12" operator="equal">
       <formula>PRESENT</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="containsText" dxfId="26" priority="22" operator="containsText" text="ABSENT">
+    <cfRule type="containsText" dxfId="47" priority="25" operator="containsText" text="ABSENT">
       <formula>NOT(ISERROR(SEARCH("ABSENT",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="PRESENT">
+    <cfRule type="containsText" dxfId="46" priority="26" operator="containsText" text="PRESENT">
       <formula>NOT(ISERROR(SEARCH("PRESENT",H2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="27" operator="equal">
       <formula>PRESENT</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:N2 C2:G6 J2:L10 C7:F7 C8:G10 M7:N10 R3:AG10 Q2:AG2 AG11:AG13">
-    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="ABSENT">
-      <formula>NOT(ISERROR(SEARCH("ABSENT",C2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="PRESENT">
-      <formula>NOT(ISERROR(SEARCH("PRESENT",C2)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="27" operator="equal">
+  <conditionalFormatting sqref="J11:N13">
+    <cfRule type="containsText" dxfId="44" priority="7" operator="containsText" text="ABSENT">
+      <formula>NOT(ISERROR(SEARCH("ABSENT",J11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="43" priority="8" operator="containsText" text="PRESENT">
+      <formula>NOT(ISERROR(SEARCH("PRESENT",J11)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="9" operator="equal">
+      <formula>PRESENT</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:O2">
+    <cfRule type="containsText" dxfId="41" priority="4" operator="containsText" text="ABSENT">
+      <formula>NOT(ISERROR(SEARCH("ABSENT",M2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="5" operator="containsText" text="PRESENT">
+      <formula>NOT(ISERROR(SEARCH("PRESENT",M2)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="6" operator="equal">
       <formula>PRESENT</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q12">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="ABSENT">
+    <cfRule type="containsText" dxfId="38" priority="13" operator="containsText" text="ABSENT">
       <formula>NOT(ISERROR(SEARCH("ABSENT",Q12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="PRESENT">
+    <cfRule type="containsText" dxfId="37" priority="14" operator="containsText" text="PRESENT">
       <formula>NOT(ISERROR(SEARCH("PRESENT",Q12)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="15" operator="equal">
       <formula>PRESENT</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13:G13 J13:L13">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="ABSENT">
-      <formula>NOT(ISERROR(SEARCH("ABSENT",C13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="PRESENT">
-      <formula>NOT(ISERROR(SEARCH("PRESENT",C13)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+  <conditionalFormatting sqref="C2:G6 J2:L10 C7:F7 M7:N10 AG11:AG13 S2:AG10">
+    <cfRule type="containsText" dxfId="35" priority="28" operator="containsText" text="ABSENT">
+      <formula>NOT(ISERROR(SEARCH("ABSENT",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="29" operator="containsText" text="PRESENT">
+      <formula>NOT(ISERROR(SEARCH("PRESENT",C2)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="30" operator="equal">
       <formula>PRESENT</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M13:N13">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="ABSENT">
-      <formula>NOT(ISERROR(SEARCH("ABSENT",M13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="PRESENT">
-      <formula>NOT(ISERROR(SEARCH("PRESENT",M13)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
-      <formula>PRESENT</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O2">
+  <conditionalFormatting sqref="Q2:R2">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="ABSENT">
-      <formula>NOT(ISERROR(SEARCH("ABSENT",O2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("ABSENT",Q2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="PRESENT">
-      <formula>NOT(ISERROR(SEARCH("PRESENT",O2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("PRESENT",Q2)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>PRESENT</formula>
@@ -1737,11 +1974,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A3D0880-F65B-45BF-ACAC-3EA58BAAB81B}">
-  <dimension ref="A1:AH12"/>
+  <dimension ref="A1:AH14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AH2" sqref="AH2"/>
+      <pane xSplit="2" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P14" sqref="P14:Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1761,6 +1998,7 @@
     <col min="14" max="14" width="19.88671875" customWidth="1"/>
     <col min="15" max="15" width="20.6640625" customWidth="1"/>
     <col min="16" max="16" width="22" customWidth="1"/>
+    <col min="17" max="17" width="22.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.3">
@@ -1912,13 +2150,16 @@
       <c r="P2" t="s">
         <v>13</v>
       </c>
+      <c r="Q2" t="s">
+        <v>13</v>
+      </c>
       <c r="AG2">
         <f>COUNTIF(C2:AF2,"PRESENT")</f>
         <v>1</v>
       </c>
       <c r="AH2">
         <f>COUNTIF(C2:AF2,"PRESENT")/COUNTA(C2:AF2)*100</f>
-        <v>8.3333333333333321</v>
+        <v>7.6923076923076925</v>
       </c>
     </row>
     <row r="3" spans="1:34" ht="27" customHeight="1" x14ac:dyDescent="0.3">
@@ -1962,9 +2203,12 @@
       <c r="P3" t="s">
         <v>12</v>
       </c>
+      <c r="Q3" t="s">
+        <v>12</v>
+      </c>
       <c r="AG3">
         <f t="shared" ref="AG3:AG12" si="0">COUNTIF(C3:AF3,"PRESENT")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AH3">
         <f t="shared" ref="AH3:AH12" si="1">COUNTIF(C3:AF3,"PRESENT")/COUNTA(C3:AF3)*100</f>
@@ -2012,13 +2256,16 @@
       <c r="P4" t="s">
         <v>13</v>
       </c>
+      <c r="Q4" t="s">
+        <v>12</v>
+      </c>
       <c r="AG4">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AH4">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>81.818181818181827</v>
       </c>
     </row>
     <row r="5" spans="1:34" ht="27" customHeight="1" x14ac:dyDescent="0.3">
@@ -2062,9 +2309,12 @@
       <c r="P5" t="s">
         <v>12</v>
       </c>
+      <c r="Q5" t="s">
+        <v>12</v>
+      </c>
       <c r="AG5">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AH5">
         <f t="shared" si="1"/>
@@ -2112,13 +2362,16 @@
       <c r="P6" t="s">
         <v>12</v>
       </c>
+      <c r="Q6" t="s">
+        <v>12</v>
+      </c>
       <c r="AG6">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AH6">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>90.909090909090907</v>
       </c>
     </row>
     <row r="7" spans="1:34" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2162,13 +2415,16 @@
       <c r="P7" t="s">
         <v>12</v>
       </c>
+      <c r="Q7" t="s">
+        <v>12</v>
+      </c>
       <c r="AG7">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AH7">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>90.909090909090907</v>
       </c>
     </row>
     <row r="8" spans="1:34" ht="27" customHeight="1" x14ac:dyDescent="0.3">
@@ -2212,6 +2468,9 @@
       <c r="P8" t="s">
         <v>13</v>
       </c>
+      <c r="Q8" t="s">
+        <v>13</v>
+      </c>
       <c r="AG8">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2262,13 +2521,16 @@
       <c r="P9" t="s">
         <v>12</v>
       </c>
+      <c r="Q9" t="s">
+        <v>12</v>
+      </c>
       <c r="AG9">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AH9">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>90.909090909090907</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.3">
@@ -2312,6 +2574,9 @@
       <c r="P10" t="s">
         <v>13</v>
       </c>
+      <c r="Q10" t="s">
+        <v>13</v>
+      </c>
       <c r="AG10">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2362,13 +2627,16 @@
       <c r="P11" t="s">
         <v>13</v>
       </c>
+      <c r="Q11" t="s">
+        <v>13</v>
+      </c>
       <c r="AG11">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AH11">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18.181818181818183</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.3">
@@ -2387,13 +2655,50 @@
       <c r="P12" t="s">
         <v>12</v>
       </c>
+      <c r="Q12" t="s">
+        <v>12</v>
+      </c>
       <c r="AG12">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH12">
         <f t="shared" si="1"/>
         <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L13" t="s">
+        <v>12</v>
+      </c>
+      <c r="M13" t="s">
+        <v>12</v>
+      </c>
+      <c r="P13" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="L14" t="s">
+        <v>12</v>
+      </c>
+      <c r="M14" t="s">
+        <v>12</v>
+      </c>
+      <c r="P14" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2401,36 +2706,102 @@
     <mergeCell ref="G2:H11"/>
     <mergeCell ref="N2:O11"/>
   </mergeCells>
-  <conditionalFormatting sqref="C2:G2 N2 I2:M11 P2:AG11 C3:F11 AG12">
-    <cfRule type="containsText" dxfId="20" priority="7" operator="containsText" text="ABSENT">
+  <conditionalFormatting sqref="C2:G2 N2 I2:M11 C3:F11 AG12 P2:AG11">
+    <cfRule type="containsText" dxfId="32" priority="25" operator="containsText" text="ABSENT">
       <formula>NOT(ISERROR(SEARCH("ABSENT",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="PRESENT">
+    <cfRule type="containsText" dxfId="31" priority="26" operator="containsText" text="PRESENT">
       <formula>NOT(ISERROR(SEARCH("PRESENT",C2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="27" operator="equal">
       <formula>PRESENT</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L12:M12">
-    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="ABSENT">
+    <cfRule type="containsText" dxfId="29" priority="19" operator="containsText" text="ABSENT">
       <formula>NOT(ISERROR(SEARCH("ABSENT",L12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="PRESENT">
+    <cfRule type="containsText" dxfId="28" priority="20" operator="containsText" text="PRESENT">
       <formula>NOT(ISERROR(SEARCH("PRESENT",L12)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="21" operator="equal">
       <formula>PRESENT</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P12">
-    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="ABSENT">
+  <conditionalFormatting sqref="P12:Q12">
+    <cfRule type="containsText" dxfId="26" priority="22" operator="containsText" text="ABSENT">
       <formula>NOT(ISERROR(SEARCH("ABSENT",P12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="PRESENT">
+    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="PRESENT">
       <formula>NOT(ISERROR(SEARCH("PRESENT",P12)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
+      <formula>PRESENT</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12:F12">
+    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="ABSENT">
+      <formula>NOT(ISERROR(SEARCH("ABSENT",C12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="PRESENT">
+      <formula>NOT(ISERROR(SEARCH("PRESENT",C12)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
+      <formula>PRESENT</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13:F13">
+    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="ABSENT">
+      <formula>NOT(ISERROR(SEARCH("ABSENT",C13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="PRESENT">
+      <formula>NOT(ISERROR(SEARCH("PRESENT",C13)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+      <formula>PRESENT</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L13:M13">
+    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="ABSENT">
+      <formula>NOT(ISERROR(SEARCH("ABSENT",L13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="PRESENT">
+      <formula>NOT(ISERROR(SEARCH("PRESENT",L13)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+      <formula>PRESENT</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L14:M14">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="ABSENT">
+      <formula>NOT(ISERROR(SEARCH("ABSENT",L14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="PRESENT">
+      <formula>NOT(ISERROR(SEARCH("PRESENT",L14)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>PRESENT</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P13:Q13">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="ABSENT">
+      <formula>NOT(ISERROR(SEARCH("ABSENT",P13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="PRESENT">
+      <formula>NOT(ISERROR(SEARCH("PRESENT",P13)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>PRESENT</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P14:Q14">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="ABSENT">
+      <formula>NOT(ISERROR(SEARCH("ABSENT",P14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="PRESENT">
+      <formula>NOT(ISERROR(SEARCH("PRESENT",P14)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>PRESENT</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2445,10 +2816,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE6D8BB-FE71-4DA4-9BDC-E79C520519E9}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2458,9 +2829,12 @@
     <col min="4" max="4" width="21.109375" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" customWidth="1"/>
     <col min="6" max="6" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>17</v>
       </c>
@@ -2474,8 +2848,17 @@
       <c r="E1" s="18">
         <v>45912</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G1" s="26">
+        <v>45913</v>
+      </c>
+      <c r="H1" s="26">
+        <v>45914</v>
+      </c>
+      <c r="I1" s="26">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -2489,8 +2872,15 @@
       <c r="E2" s="11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G2" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="19"/>
+      <c r="I2" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="21" t="s">
         <v>21</v>
       </c>
@@ -2504,8 +2894,13 @@
       <c r="E3" s="11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="21" t="s">
         <v>22</v>
       </c>
@@ -2520,8 +2915,13 @@
         <v>20</v>
       </c>
       <c r="F4" s="11"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="21" t="s">
         <v>23</v>
       </c>
@@ -2535,8 +2935,13 @@
       <c r="E5" s="10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="21" t="s">
         <v>24</v>
       </c>
@@ -2550,8 +2955,13 @@
       <c r="E6" s="10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="23" t="s">
         <v>25</v>
       </c>
@@ -2565,9 +2975,65 @@
       <c r="E7" s="11" t="s">
         <v>20</v>
       </c>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="10">
+    <mergeCell ref="G2:H11"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A1:B1"/>
@@ -2576,8 +3042,23 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
   </mergeCells>
+  <conditionalFormatting sqref="G2">
+    <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="ABSENT">
+      <formula>NOT(ISERROR(SEARCH("ABSENT",G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="PRESENT">
+      <formula>NOT(ISERROR(SEARCH("PRESENT",G2)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
+      <formula>PRESENT</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="A8" r:id="rId1" xr:uid="{A1493653-08FB-42D5-8819-059233FC147E}"/>
+    <hyperlink ref="A9" r:id="rId2" xr:uid="{DBA9D027-5522-4753-ABAE-14AE233AE492}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>